<commit_message>
Added client report and report page to owner
</commit_message>
<xml_diff>
--- a/core/src/main/resources/exceltemplates/profit report.xlsx
+++ b/core/src/main/resources/exceltemplates/profit report.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\#download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\iTechArtGroup Java Lab\onlinewarehouse\core\src\main\resources\exceltemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="chartsheet" sheetId="4" r:id="rId1"/>
@@ -29,21 +29,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Mount</t>
   </si>
   <si>
     <t>Profit</t>
-  </si>
-  <si>
-    <t>2018-12</t>
-  </si>
-  <si>
-    <t>2018-11</t>
-  </si>
-  <si>
-    <t>2018-10</t>
   </si>
   <si>
     <t>№</t>
@@ -248,15 +239,13 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>[0]!mount</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2018-12</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -264,9 +253,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>700</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1017,7 +1003,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1028,7 +1014,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9300427" cy="6078963"/>
+    <xdr:ext cx="9308171" cy="6078963"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Диаграмма 1"/>
@@ -1314,17 +1300,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C6"/>
+  <dimension ref="A3:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1333,30 +1319,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>136</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>